<commit_message>
Modified the excel data
</commit_message>
<xml_diff>
--- a/HealthRecordAutomation/TestData/open_emr_data.xlsx
+++ b/HealthRecordAutomation/TestData/open_emr_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\Sileverlake Malaysia July 2024\AutomationFrameworkSolution\HealthRecordAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2035919-6938-4A8D-9FAA-97C57CB655E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9477B245-9C9B-4F3E-87DE-365DEDFF986B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5486" yWindow="2014" windowWidth="16457" windowHeight="9549" activeTab="1" xr2:uid="{DF20F66C-A67A-417F-8B1D-36F638E4EB22}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" activeTab="1" xr2:uid="{DF20F66C-A67A-417F-8B1D-36F638E4EB22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>Invalid username or password</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -467,10 +461,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703EB5DD-0646-4F11-89EC-FEA7910C85E2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -509,17 +503,6 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>